<commit_message>
eddy ni 1978-1979 (update)
</commit_message>
<xml_diff>
--- a/_data/ni/ni7879/individueel_eindstand_dworp_12_7879.xlsx
+++ b/_data/ni/ni7879/individueel_eindstand_dworp_12_7879.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="-15" yWindow="-15" windowWidth="14355" windowHeight="12870"/>
-    <workbookView xWindow="14355" yWindow="-15" windowWidth="14385" windowHeight="12870" activeTab="11"/>
+    <workbookView xWindow="14355" yWindow="-15" windowWidth="14385" windowHeight="12870" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1269" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1271" uniqueCount="177">
   <si>
     <t>Jaar 1</t>
   </si>
@@ -305,9 +305,6 @@
     <t>Maes E</t>
   </si>
   <si>
-    <t>Van den Heeden A</t>
-  </si>
-  <si>
     <t>Coorevits Y</t>
   </si>
   <si>
@@ -533,12 +530,6 @@
     <t>matchpunten: w 3 - g 2 - v 1 - vf 0</t>
   </si>
   <si>
-    <t>17?</t>
-  </si>
-  <si>
-    <t>13?</t>
-  </si>
-  <si>
     <t>402 Jean Jaurès Gent 5</t>
   </si>
   <si>
@@ -546,6 +537,38 @@
   </si>
   <si>
     <t>4E</t>
+  </si>
+  <si>
+    <t>Van den Heede A</t>
+  </si>
+  <si>
+    <t>15?</t>
+  </si>
+  <si>
+    <t>12?</t>
+  </si>
+  <si>
+    <t>19?</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Dworp 2 - </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>rooster identiek aan Eddy zijn notities</t>
+    </r>
+  </si>
+  <si>
+    <t>5? of 81?</t>
+  </si>
+  <si>
+    <t>11? of 77?</t>
   </si>
 </sst>
 </file>
@@ -1179,7 +1202,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="92">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1413,11 +1436,14 @@
     <xf numFmtId="0" fontId="10" fillId="13" borderId="18" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="165" fontId="10" fillId="13" borderId="17" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="16" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -1759,11 +1785,11 @@
         <v>1</v>
       </c>
       <c r="B5" s="68" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C5" s="63"/>
       <c r="D5" s="63" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E5" s="63"/>
       <c r="F5" s="63"/>
@@ -1774,7 +1800,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="69" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="7" spans="1:7">
@@ -1791,13 +1817,13 @@
     </row>
     <row r="9" spans="1:7" ht="15.75" thickBot="1">
       <c r="A9" s="71" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B9" s="72"/>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="73" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B10" s="74">
         <v>0</v>
@@ -1805,7 +1831,7 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="73" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B11" s="75">
         <v>0</v>
@@ -1813,7 +1839,7 @@
     </row>
     <row r="12" spans="1:7" ht="15.75" thickBot="1">
       <c r="A12" s="73" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B12" s="76">
         <v>1</v>
@@ -1898,7 +1924,7 @@
         <v>12</v>
       </c>
       <c r="I3" s="15" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="J3" s="1"/>
     </row>
@@ -1956,7 +1982,7 @@
       </c>
       <c r="H5" s="19"/>
       <c r="I5" s="14" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J5" s="18"/>
     </row>
@@ -1984,7 +2010,7 @@
       </c>
       <c r="H6" s="19"/>
       <c r="I6" s="14" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J6" s="18"/>
     </row>
@@ -2012,7 +2038,7 @@
       </c>
       <c r="H7" s="19"/>
       <c r="I7" s="14" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="J7" s="18"/>
     </row>
@@ -2040,7 +2066,7 @@
       </c>
       <c r="H8" s="19"/>
       <c r="I8" s="14" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J8" s="18"/>
     </row>
@@ -2121,7 +2147,7 @@
         <v>11</v>
       </c>
       <c r="I13" s="15" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="J13" s="1"/>
     </row>
@@ -2179,7 +2205,7 @@
       </c>
       <c r="H15" s="19"/>
       <c r="I15" s="14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="J15" s="18"/>
     </row>
@@ -2207,7 +2233,7 @@
       </c>
       <c r="H16" s="19"/>
       <c r="I16" s="14" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="J16" s="18"/>
     </row>
@@ -2219,7 +2245,7 @@
         <v>52</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D17" s="18">
         <v>1173</v>
@@ -2235,7 +2261,7 @@
       </c>
       <c r="H17" s="19"/>
       <c r="I17" s="14" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="J17" s="18"/>
     </row>
@@ -2263,7 +2289,7 @@
       </c>
       <c r="H18" s="19"/>
       <c r="I18" s="14" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="J18" s="18"/>
     </row>
@@ -2611,7 +2637,7 @@
         <v>12</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -2661,7 +2687,7 @@
       </c>
       <c r="B5" s="19"/>
       <c r="C5" s="14" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D5" s="18"/>
       <c r="E5" s="10">
@@ -2689,7 +2715,7 @@
       </c>
       <c r="B6" s="19"/>
       <c r="C6" s="14" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D6" s="18"/>
       <c r="E6" s="10">
@@ -2717,7 +2743,7 @@
       </c>
       <c r="B7" s="19"/>
       <c r="C7" s="14" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D7" s="18"/>
       <c r="E7" s="10">
@@ -2745,7 +2771,7 @@
       </c>
       <c r="B8" s="19"/>
       <c r="C8" s="14" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D8" s="18"/>
       <c r="E8" s="10">
@@ -2834,7 +2860,7 @@
         <v>11</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -2884,7 +2910,7 @@
       </c>
       <c r="B15" s="19"/>
       <c r="C15" s="14" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D15" s="18"/>
       <c r="E15" s="10">
@@ -2912,7 +2938,7 @@
       </c>
       <c r="B16" s="19"/>
       <c r="C16" s="14" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D16" s="18"/>
       <c r="E16" s="10">
@@ -2928,7 +2954,7 @@
         <v>52</v>
       </c>
       <c r="I16" s="14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J16" s="18">
         <v>1173</v>
@@ -2940,7 +2966,7 @@
       </c>
       <c r="B17" s="19"/>
       <c r="C17" s="14" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D17" s="18"/>
       <c r="E17" s="10">
@@ -2968,7 +2994,7 @@
       </c>
       <c r="B18" s="19"/>
       <c r="C18" s="14" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D18" s="18"/>
       <c r="E18" s="12">
@@ -3295,7 +3321,7 @@
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView tabSelected="1" workbookViewId="1"/>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -3906,9 +3932,7 @@
     <sheetView workbookViewId="0">
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
-    <sheetView workbookViewId="1">
-      <selection activeCell="R28" sqref="R28"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -3937,13 +3961,13 @@
         <v>14</v>
       </c>
       <c r="S2" s="77" t="s">
+        <v>164</v>
+      </c>
+      <c r="AF2" s="78" t="s">
         <v>165</v>
       </c>
-      <c r="AF2" s="78" t="s">
+      <c r="AS2" s="77" t="s">
         <v>166</v>
-      </c>
-      <c r="AS2" s="77" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="3" spans="1:56" s="43" customFormat="1" ht="16.5" thickTop="1" thickBot="1">
@@ -4224,7 +4248,7 @@
         <v>2</v>
       </c>
       <c r="B5" s="32" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C5" s="34">
         <v>7</v>
@@ -4420,7 +4444,7 @@
         <v>3</v>
       </c>
       <c r="B6" s="32" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C6" s="34">
         <v>6</v>
@@ -4616,7 +4640,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="32" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C7" s="34">
         <v>9</v>
@@ -4812,7 +4836,7 @@
         <v>5</v>
       </c>
       <c r="B8" s="32" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C8" s="34">
         <v>4</v>
@@ -5400,7 +5424,7 @@
         <v>8</v>
       </c>
       <c r="B11" s="32" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C11" s="34">
         <v>6</v>
@@ -5596,7 +5620,7 @@
         <v>9</v>
       </c>
       <c r="B12" s="32" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C12" s="34">
         <v>6</v>
@@ -5792,7 +5816,7 @@
         <v>10</v>
       </c>
       <c r="B13" s="32" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C13" s="34">
         <v>6</v>
@@ -6355,7 +6379,7 @@
     </row>
     <row r="16" spans="1:56" s="43" customFormat="1" ht="16.5" thickTop="1" thickBot="1">
       <c r="A16" s="59" t="s">
-        <v>15</v>
+        <v>174</v>
       </c>
       <c r="S16" s="60"/>
       <c r="T16" s="60"/>
@@ -6452,7 +6476,7 @@
         <v>1</v>
       </c>
       <c r="B18" s="32" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C18" s="33" t="s">
         <v>37</v>
@@ -6648,7 +6672,7 @@
         <v>2</v>
       </c>
       <c r="B19" s="32" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C19" s="34">
         <v>9</v>
@@ -6844,7 +6868,7 @@
         <v>3</v>
       </c>
       <c r="B20" s="32" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C20" s="34">
         <v>6</v>
@@ -7040,7 +7064,7 @@
         <v>4</v>
       </c>
       <c r="B21" s="32" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C21" s="34">
         <v>7</v>
@@ -7455,7 +7479,7 @@
       <c r="I23" s="34">
         <v>10</v>
       </c>
-      <c r="J23" s="34">
+      <c r="J23" s="91">
         <v>6</v>
       </c>
       <c r="K23" s="34">
@@ -7468,9 +7492,8 @@
         <v>12</v>
       </c>
       <c r="N23" s="34"/>
-      <c r="O23" s="35">
-        <f t="shared" si="6"/>
-        <v>81</v>
+      <c r="O23" s="90">
+        <v>80</v>
       </c>
       <c r="P23" s="36">
         <f>IF(Info!B$10=0,0,SUM(S23:AD23))+IF(Info!B$11=0,0,2*SUM(S23:AD23))+IF(Info!B$12=0,0,SUM(AS23:BD23))</f>
@@ -7480,7 +7503,9 @@
         <f t="shared" si="7"/>
         <v>10</v>
       </c>
-      <c r="R23" s="45"/>
+      <c r="R23" s="89" t="s">
+        <v>175</v>
+      </c>
       <c r="S23" s="47">
         <f>IF(C23="","",IF(C23&gt;$H18,1,IF(C23=$H18,0.5,0)))</f>
         <v>0</v>
@@ -7628,7 +7653,7 @@
         <v>7</v>
       </c>
       <c r="B24" s="32" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C24" s="34">
         <v>8</v>
@@ -7669,15 +7694,14 @@
         <v>80</v>
       </c>
       <c r="P24" s="88">
-        <f>IF(Info!B$10=0,0,SUM(S24:AD24))+IF(Info!B$11=0,0,2*SUM(S24:AD24))+IF(Info!B$12=0,0,SUM(AS24:BD24))</f>
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="Q24" s="36">
         <f t="shared" si="7"/>
         <v>10</v>
       </c>
-      <c r="R24" s="90" t="s">
-        <v>168</v>
+      <c r="R24" s="89" t="s">
+        <v>173</v>
       </c>
       <c r="S24" s="47">
         <f>IF(C24="","",IF(C24&gt;$I18,1,IF(C24=$I18,0.5,0)))</f>
@@ -7826,7 +7850,7 @@
         <v>8</v>
       </c>
       <c r="B25" s="32" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C25" s="34">
         <v>4</v>
@@ -7843,7 +7867,7 @@
       <c r="G25" s="34">
         <v>9</v>
       </c>
-      <c r="H25" s="34">
+      <c r="H25" s="91">
         <v>10</v>
       </c>
       <c r="I25" s="34">
@@ -7862,9 +7886,8 @@
         <v>11</v>
       </c>
       <c r="N25" s="34"/>
-      <c r="O25" s="35">
-        <f t="shared" si="6"/>
-        <v>77</v>
+      <c r="O25" s="90">
+        <v>78</v>
       </c>
       <c r="P25" s="36">
         <f>IF(Info!B$10=0,0,SUM(S25:AD25))+IF(Info!B$11=0,0,2*SUM(S25:AD25))+IF(Info!B$12=0,0,SUM(AS25:BD25))</f>
@@ -7874,7 +7897,9 @@
         <f t="shared" si="7"/>
         <v>10</v>
       </c>
-      <c r="R25" s="89"/>
+      <c r="R25" s="89" t="s">
+        <v>176</v>
+      </c>
       <c r="S25" s="47">
         <f>IF(C25="","",IF(C25&gt;$J18,1,IF(C25=$J18,0.5,0)))</f>
         <v>0</v>
@@ -8022,7 +8047,7 @@
         <v>9</v>
       </c>
       <c r="B26" s="32" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C26" s="34">
         <v>5</v>
@@ -8063,15 +8088,14 @@
         <v>69</v>
       </c>
       <c r="P26" s="88">
-        <f>IF(Info!B$10=0,0,SUM(S26:AD26))+IF(Info!B$11=0,0,2*SUM(S26:AD26))+IF(Info!B$12=0,0,SUM(AS26:BD26))</f>
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="Q26" s="36">
         <f t="shared" si="7"/>
         <v>10</v>
       </c>
-      <c r="R26" s="90" t="s">
-        <v>169</v>
+      <c r="R26" s="89" t="s">
+        <v>171</v>
       </c>
       <c r="S26" s="47">
         <f>IF(C26="","",IF(C26&gt;$K18,1,IF(C26=$K18,0.5,0)))</f>
@@ -8261,15 +8285,14 @@
         <v>56</v>
       </c>
       <c r="P27" s="88">
-        <f>IF(Info!B$10=0,0,SUM(S27:AD27))+IF(Info!B$11=0,0,2*SUM(S27:AD27))+IF(Info!B$12=0,0,SUM(AS27:BD27))</f>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="Q27" s="36">
         <f t="shared" si="7"/>
         <v>10</v>
       </c>
-      <c r="R27" s="90" t="s">
-        <v>169</v>
+      <c r="R27" s="89" t="s">
+        <v>172</v>
       </c>
       <c r="S27" s="47">
         <f>IF(C27="","",IF(C27&gt;$L18,1,IF(C27=$L18,0.5,0)))</f>
@@ -8418,7 +8441,7 @@
         <v>11</v>
       </c>
       <c r="B28" s="32" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C28" s="34">
         <v>3</v>
@@ -16551,7 +16574,7 @@
         <v>12</v>
       </c>
       <c r="I13" s="15" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="J13" s="1"/>
     </row>
@@ -17776,7 +17799,7 @@
         <v>12</v>
       </c>
       <c r="I3" s="15" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="J3" s="1"/>
     </row>
@@ -17999,7 +18022,7 @@
         <v>12</v>
       </c>
       <c r="I13" s="15" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="J13" s="1"/>
     </row>
@@ -18450,7 +18473,9 @@
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="1">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -18712,7 +18737,7 @@
         <v>11</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -18726,7 +18751,7 @@
       </c>
       <c r="J13" s="1"/>
       <c r="L13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="14" spans="1:12">
@@ -18821,7 +18846,7 @@
       </c>
       <c r="B17" s="19"/>
       <c r="C17" s="14" t="s">
-        <v>92</v>
+        <v>170</v>
       </c>
       <c r="D17" s="18"/>
       <c r="E17" s="10">
@@ -18837,7 +18862,7 @@
         <v>52</v>
       </c>
       <c r="I17" s="14" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J17" s="18">
         <v>1173</v>
@@ -18849,7 +18874,7 @@
       </c>
       <c r="B18" s="19"/>
       <c r="C18" s="14" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D18" s="18"/>
       <c r="E18" s="12">
@@ -19215,7 +19240,7 @@
         <v>11</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -19265,7 +19290,7 @@
       </c>
       <c r="B5" s="19"/>
       <c r="C5" s="14" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D5" s="18"/>
       <c r="E5" s="10">
@@ -19293,7 +19318,7 @@
       </c>
       <c r="B6" s="19"/>
       <c r="C6" s="14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D6" s="18"/>
       <c r="E6" s="10">
@@ -19321,7 +19346,7 @@
       </c>
       <c r="B7" s="19"/>
       <c r="C7" s="14" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D7" s="18"/>
       <c r="E7" s="10">
@@ -19349,7 +19374,7 @@
       </c>
       <c r="B8" s="19"/>
       <c r="C8" s="14" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D8" s="18"/>
       <c r="E8" s="10">
@@ -19438,7 +19463,7 @@
         <v>11</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -19488,7 +19513,7 @@
       </c>
       <c r="B15" s="19"/>
       <c r="C15" s="14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D15" s="18"/>
       <c r="E15" s="10">
@@ -19516,7 +19541,7 @@
       </c>
       <c r="B16" s="19"/>
       <c r="C16" s="14" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D16" s="18"/>
       <c r="E16" s="10">
@@ -19544,7 +19569,7 @@
       </c>
       <c r="B17" s="19"/>
       <c r="C17" s="14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D17" s="18"/>
       <c r="E17" s="10">
@@ -19572,7 +19597,7 @@
       </c>
       <c r="B18" s="19"/>
       <c r="C18" s="14" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D18" s="18"/>
       <c r="E18" s="12">
@@ -19950,7 +19975,7 @@
         <v>12</v>
       </c>
       <c r="I3" s="15" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="J3" s="1"/>
     </row>
@@ -20008,7 +20033,7 @@
       </c>
       <c r="H5" s="19"/>
       <c r="I5" s="14" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="J5" s="18"/>
     </row>
@@ -20036,7 +20061,7 @@
       </c>
       <c r="H6" s="19"/>
       <c r="I6" s="14" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J6" s="18"/>
     </row>
@@ -20064,7 +20089,7 @@
       </c>
       <c r="H7" s="19"/>
       <c r="I7" s="14" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="J7" s="18"/>
     </row>
@@ -20092,7 +20117,7 @@
       </c>
       <c r="H8" s="19"/>
       <c r="I8" s="14" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="J8" s="18"/>
     </row>
@@ -20177,7 +20202,7 @@
       </c>
       <c r="J13" s="1"/>
       <c r="L13" s="63" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="M13" s="63"/>
     </row>
@@ -20219,7 +20244,7 @@
         <v>57282</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D15" s="18">
         <v>1245</v>
@@ -20235,7 +20260,7 @@
       </c>
       <c r="H15" s="19"/>
       <c r="I15" s="14" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J15" s="18"/>
     </row>
@@ -20263,7 +20288,7 @@
       </c>
       <c r="H16" s="19"/>
       <c r="I16" s="14" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="J16" s="18"/>
     </row>
@@ -20291,7 +20316,7 @@
       </c>
       <c r="H17" s="19"/>
       <c r="I17" s="14" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="J17" s="18"/>
     </row>
@@ -20303,7 +20328,7 @@
         <v>64327</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D18" s="18">
         <v>807</v>
@@ -20319,7 +20344,7 @@
       </c>
       <c r="H18" s="19"/>
       <c r="I18" s="14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="J18" s="18"/>
     </row>
@@ -20667,7 +20692,7 @@
         <v>12</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -20717,7 +20742,7 @@
       </c>
       <c r="B5" s="19"/>
       <c r="C5" s="14" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D5" s="18"/>
       <c r="E5" s="10">
@@ -20745,7 +20770,7 @@
       </c>
       <c r="B6" s="19"/>
       <c r="C6" s="14" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D6" s="18"/>
       <c r="E6" s="10">
@@ -20773,7 +20798,7 @@
       </c>
       <c r="B7" s="19"/>
       <c r="C7" s="14" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D7" s="18"/>
       <c r="E7" s="10">
@@ -20801,7 +20826,7 @@
       </c>
       <c r="B8" s="19"/>
       <c r="C8" s="14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D8" s="18"/>
       <c r="E8" s="10">
@@ -20890,7 +20915,7 @@
         <v>11</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
@@ -20940,7 +20965,7 @@
       </c>
       <c r="B15" s="19"/>
       <c r="C15" s="14" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D15" s="18"/>
       <c r="E15" s="10">
@@ -20968,7 +20993,7 @@
       </c>
       <c r="B16" s="19"/>
       <c r="C16" s="14" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="D16" s="18"/>
       <c r="E16" s="10">
@@ -20996,7 +21021,7 @@
       </c>
       <c r="B17" s="19"/>
       <c r="C17" s="14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D17" s="18"/>
       <c r="E17" s="10">
@@ -21024,7 +21049,7 @@
       </c>
       <c r="B18" s="19"/>
       <c r="C18" s="14" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D18" s="18"/>
       <c r="E18" s="12">
@@ -21402,7 +21427,7 @@
         <v>12</v>
       </c>
       <c r="I3" s="15" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="J3" s="1"/>
     </row>
@@ -21460,7 +21485,7 @@
       </c>
       <c r="H5" s="19"/>
       <c r="I5" s="14" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="J5" s="18"/>
     </row>
@@ -21488,7 +21513,7 @@
       </c>
       <c r="H6" s="19"/>
       <c r="I6" s="14" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="J6" s="18"/>
     </row>
@@ -21516,7 +21541,7 @@
       </c>
       <c r="H7" s="19"/>
       <c r="I7" s="14" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J7" s="18"/>
     </row>
@@ -21544,7 +21569,7 @@
       </c>
       <c r="H8" s="19"/>
       <c r="I8" s="14" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="J8" s="18"/>
     </row>
@@ -21625,7 +21650,7 @@
         <v>12</v>
       </c>
       <c r="I13" s="15" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="J13" s="1"/>
     </row>
@@ -21683,7 +21708,7 @@
       </c>
       <c r="H15" s="19"/>
       <c r="I15" s="14" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J15" s="18"/>
     </row>
@@ -21711,7 +21736,7 @@
       </c>
       <c r="H16" s="19"/>
       <c r="I16" s="14" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="J16" s="18"/>
     </row>
@@ -21739,11 +21764,11 @@
       </c>
       <c r="H17" s="19"/>
       <c r="I17" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J17" s="18"/>
       <c r="L17" s="63" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="M17" s="63"/>
       <c r="N17" s="63"/>
@@ -21775,7 +21800,7 @@
       </c>
       <c r="H18" s="19"/>
       <c r="I18" s="14" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="J18" s="18"/>
     </row>

</xml_diff>

<commit_message>
eddy ni 1978-1979 (update 2)
</commit_message>
<xml_diff>
--- a/_data/ni/ni7879/individueel_eindstand_dworp_12_7879.xlsx
+++ b/_data/ni/ni7879/individueel_eindstand_dworp_12_7879.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="-15" yWindow="-15" windowWidth="14355" windowHeight="12870"/>
-    <workbookView xWindow="14355" yWindow="-15" windowWidth="14385" windowHeight="12870" activeTab="12"/>
+    <workbookView xWindow="14355" yWindow="-15" windowWidth="14385" windowHeight="12870"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -1749,7 +1749,7 @@
   <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
+    <sheetView tabSelected="1" workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -3932,7 +3932,7 @@
     <sheetView workbookViewId="0">
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
-    <sheetView tabSelected="1" workbookViewId="1"/>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -18473,8 +18473,8 @@
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView topLeftCell="C1" workbookViewId="1">
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -18850,13 +18850,13 @@
       </c>
       <c r="D17" s="18"/>
       <c r="E17" s="10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F17" s="10" t="s">
         <v>10</v>
       </c>
       <c r="G17" s="10">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H17" s="19" t="s">
         <v>52</v>
@@ -18878,13 +18878,13 @@
       </c>
       <c r="D18" s="18"/>
       <c r="E18" s="12">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F18" s="10" t="s">
         <v>10</v>
       </c>
       <c r="G18" s="12">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H18" s="19">
         <v>76317</v>
@@ -18905,13 +18905,13 @@
       </c>
       <c r="D19" s="3"/>
       <c r="E19" s="13">
+        <v>10</v>
+      </c>
+      <c r="F19" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="G19" s="13">
         <v>6</v>
-      </c>
-      <c r="F19" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="G19" s="13">
-        <v>10</v>
       </c>
       <c r="H19" s="3"/>
       <c r="I19" s="16">

</xml_diff>

<commit_message>
conversatie in excel ni 78-99
</commit_message>
<xml_diff>
--- a/_data/ni/ni7879/individueel_eindstand_dworp_12_7879.xlsx
+++ b/_data/ni/ni7879/individueel_eindstand_dworp_12_7879.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\meneer\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{0AF86B15-ACF3-43FA-AFDA-246D1E612A92}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{90B03022-B643-4C51-84C4-F4E34821D1F8}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="11508" windowHeight="7812" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1412" uniqueCount="272">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1484" uniqueCount="329">
   <si>
     <t>Jaar 1</t>
   </si>
@@ -851,9 +851,6 @@
     <t>DEEL 1</t>
   </si>
   <si>
-    <t>zo 6 jan. 2018</t>
-  </si>
-  <si>
     <t>ng</t>
   </si>
   <si>
@@ -861,6 +858,192 @@
   </si>
   <si>
     <t>V</t>
+  </si>
+  <si>
+    <t>Dag Herman,</t>
+  </si>
+  <si>
+    <t>In de bijlage op het eerste en tweede tabblad staat uitvoerig beschreven dat Dworp die eerste ronde wel zal bye geweest zijn zoals jij aantoont.</t>
+  </si>
+  <si>
+    <t>Daarna is het wat uit de hand gelopen met een naadloze overgang naar mijn memoires. Ik was toen nog helder van geest…</t>
+  </si>
+  <si>
+    <t>Veel plezier met de anekdotes, het is niet eens een cursiefje.</t>
+  </si>
+  <si>
+    <t>Groetjes en vooral hartelijk dank om ons seizoen 1978-1979 te fine-tunen,</t>
+  </si>
+  <si>
+    <t>zo 6 jan. 2019 18:58</t>
+  </si>
+  <si>
+    <t>zo 6 jan. 2019 19:07</t>
+  </si>
+  <si>
+    <t>Dag Pieter en Diederik,</t>
+  </si>
+  <si>
+    <t>Op de bijlage vinden jullie alle juiste datums bij de juiste ronden.</t>
+  </si>
+  <si>
+    <t>In ronde 4 speelde Luc Vandermeersch ng (niet 1136); het gemiddelde ploegtotaal is dan 1210.</t>
+  </si>
+  <si>
+    <t>In ronde 11 speelde Luc Vandermeersch ng (niet 1136); het gemiddelde ploegtotaal is dan 1212.</t>
+  </si>
+  <si>
+    <t>Herman</t>
+  </si>
+  <si>
+    <t>Bij het opruimen van mijn papieren ben ik op een document gevallen. Zie bijlage. Document KGSRL.</t>
+  </si>
+  <si>
+    <t>In het seizoen 1978-79 in reeks 4D waren er elf ploegen, waarvan één bye. Toevallig ronde 1.</t>
+  </si>
+  <si>
+    <t>za 1 dec. 2018 14:48</t>
+  </si>
+  <si>
+    <t>Van de Wynkele Herman</t>
+  </si>
+  <si>
+    <t>herman.senior@belgacom.net</t>
+  </si>
+  <si>
+    <t>Eerste ronde: 22-10-1978 Dworp bye</t>
+  </si>
+  <si>
+    <t>waarschijnlijk laatste ronde 18-03-1979 (25-03-1979 is foutief)</t>
+  </si>
+  <si>
+    <t>wo 19 dec. 2018 17:21</t>
+  </si>
+  <si>
+    <t>Mijn geheugen is niet meer van het beste; ik weet niet meer wanneer ik wát, bijvoorbeeld, in 1980 heb uitgespookt.</t>
+  </si>
+  <si>
+    <t>Daarentegen, de maand maart van het fantastische jaar 1979 waarover je mailt ... die ligt nog vers in het geheugen.</t>
+  </si>
+  <si>
+    <t>In februari werd ik soldaat en een maand later werd ik overgeplaatst naar Duitsland,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">naar het onooglijke Arolsen voor de kenners onder ons. </t>
+  </si>
+  <si>
+    <t>De NIC-uitslagen van 1979 heb ik moeten verzamelen zo goed en zo kwaad als het ging.</t>
+  </si>
+  <si>
+    <t>Ik gok daarbij op de bondsbladen van (Alex?) Vermandel.</t>
+  </si>
+  <si>
+    <t>Afijn, ik zal mijn archief eens vergelijken met wat de website van onze kring te bieden heeft. Geef je mij daarvoor wat tijd?</t>
+  </si>
+  <si>
+    <t>ma 31 dec. 2018 17:20</t>
+  </si>
+  <si>
+    <t>Na een reeks berekeningen ben ik opnieuw tot de conclusie gekomen dat dit vraagstuk onoplosbaar is met wiskunde en logica.</t>
+  </si>
+  <si>
+    <t>Ik heb echter wel een sterk argument om te poneren dat de eerste ronde van het seizoen 1978-1979 op 22 oktober 1978 werd betwist.</t>
+  </si>
+  <si>
+    <t>Hoe kom jij eigenlijk aan die datum? Het je bijvoorbeeld een notatieformulier met die datum?</t>
+  </si>
+  <si>
+    <t>Een visioen gekregen? In de Informator gevonden? …</t>
+  </si>
+  <si>
+    <t>di 1 jan. 2019 03:54</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dus: </t>
+  </si>
+  <si>
+    <t>Ronde 01
+22-10-1978</t>
+  </si>
+  <si>
+    <t>Ronde 01 22-10-1978</t>
+  </si>
+  <si>
+    <t>Ronde 02
+05-11-1978</t>
+  </si>
+  <si>
+    <t>Ronde 03
+19-11-1978</t>
+  </si>
+  <si>
+    <t>Ronde 04
+03-12-1978</t>
+  </si>
+  <si>
+    <t>Ronde 05
+07-01-1979</t>
+  </si>
+  <si>
+    <t>Ronde 06
+28-01-1979</t>
+  </si>
+  <si>
+    <t>Ronde 07
+11-02-1979</t>
+  </si>
+  <si>
+    <t>Ronde 08
+25-02-1979</t>
+  </si>
+  <si>
+    <t>Ronde 09
+04-03-1979</t>
+  </si>
+  <si>
+    <t>Ronde 10
+11-03-1979</t>
+  </si>
+  <si>
+    <t>Ronde 11
+25-03-1979</t>
+  </si>
+  <si>
+    <t>In facto begint u met ronde 2 als ronde 1 vermeld.</t>
+  </si>
+  <si>
+    <t>Dat is alles Eddy.</t>
+  </si>
+  <si>
+    <t>Mijn partijen die ik heb gevonden of beter gespeeld heb:</t>
+  </si>
+  <si>
+    <t>Hier heb ik 21-01-1979 als zesde ronde, en 18-03-1979 als  ?, maar ik betwist niet deze</t>
+  </si>
+  <si>
+    <t>data. Tenslotte lijkt me 11-03-1979 of 25-03-1979 logischer.</t>
+  </si>
+  <si>
+    <t>Alleen het uittreksel voor ronde 1.</t>
+  </si>
+  <si>
+    <t>Eddy, ik hoop hiermede te helpen, want fouten zijn rap gemaakt ook door mij.</t>
+  </si>
+  <si>
+    <t>Daar ik alles aan het opruimen ben, heb ik waarschijnlijk al mijn notatieformulieren weggegooid.</t>
+  </si>
+  <si>
+    <t>Om de juiste data te achterhalen als neutraal zal ik de voorzitter van MSV aanspreken om in de archieven van MSV te kijken.</t>
+  </si>
+  <si>
+    <t>Ronde 06
+21-01-1979</t>
+  </si>
+  <si>
+    <t>Ronde ?? 18-03-1979</t>
+  </si>
+  <si>
+    <t>zo 6 jan. 2019</t>
   </si>
 </sst>
 </file>
@@ -871,7 +1054,7 @@
     <numFmt numFmtId="164" formatCode="d/mm/yyyy;@"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="16" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -982,6 +1165,14 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="18">
@@ -1576,12 +1767,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="124">
+  <cellXfs count="127">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1872,8 +2064,12 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
     <cellStyle name="Standaard 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
     <cellStyle name="Standaard_Blad2" xfId="2" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
@@ -2212,9 +2408,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G46"/>
+  <dimension ref="A1:P106"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A93" sqref="A93"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2472,43 +2670,483 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>268</v>
+        <v>285</v>
       </c>
       <c r="B41" t="s">
-        <v>178</v>
+        <v>282</v>
       </c>
       <c r="C41" t="s">
-        <v>204</v>
+        <v>286</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C42" t="s">
-        <v>205</v>
+      <c r="C42" s="124" t="s">
+        <v>287</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C43" t="s">
-        <v>206</v>
+        <v>288</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C44" t="s">
-        <v>207</v>
+        <v>289</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>290</v>
+      </c>
+      <c r="B45" t="s">
+        <v>178</v>
+      </c>
       <c r="C45" t="s">
-        <v>208</v>
+        <v>291</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="C46" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C47" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C48" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C49" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C50" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C51" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>298</v>
+      </c>
+      <c r="B52" t="s">
+        <v>178</v>
+      </c>
+      <c r="C52" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C53" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C54" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C55" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>303</v>
+      </c>
+      <c r="B56" t="s">
+        <v>282</v>
+      </c>
+      <c r="C56" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C57" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C58" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C59" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C60" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C61" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C62" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C63" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C64" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="65" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C65" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="66" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C66" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="67" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C67" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="68" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C68" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="69" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C69" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="70" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C70" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="71" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C71" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="72" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C72" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="73" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C73" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="74" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C74" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="75" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C75" s="125" t="s">
+        <v>322</v>
+      </c>
+      <c r="D75" s="125"/>
+      <c r="E75" s="125"/>
+      <c r="F75" s="125"/>
+    </row>
+    <row r="76" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C76" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="77" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C77" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="78" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C78" s="125" t="s">
+        <v>325</v>
+      </c>
+      <c r="D78" s="125"/>
+      <c r="E78" s="125"/>
+      <c r="F78" s="125"/>
+      <c r="G78" s="125"/>
+      <c r="H78" s="125"/>
+      <c r="I78" s="125"/>
+      <c r="J78" s="125"/>
+      <c r="K78" s="125"/>
+      <c r="L78" s="125"/>
+      <c r="M78" s="125"/>
+      <c r="N78" s="125"/>
+    </row>
+    <row r="79" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C79" s="63" t="s">
+        <v>305</v>
+      </c>
+      <c r="D79" s="63"/>
+    </row>
+    <row r="80" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C80" s="63" t="s">
+        <v>307</v>
+      </c>
+      <c r="D80" s="63"/>
+    </row>
+    <row r="81" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="C81" s="63" t="s">
+        <v>308</v>
+      </c>
+      <c r="D81" s="63"/>
+    </row>
+    <row r="82" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="C82" s="63" t="s">
+        <v>309</v>
+      </c>
+      <c r="D82" s="63"/>
+    </row>
+    <row r="83" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="C83" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="84" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="C84" s="63" t="s">
+        <v>326</v>
+      </c>
+      <c r="D84" s="63"/>
+    </row>
+    <row r="85" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="C85" s="126" t="s">
+        <v>311</v>
+      </c>
+      <c r="D85" s="126"/>
+    </row>
+    <row r="86" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="C86" s="63" t="s">
+        <v>312</v>
+      </c>
+      <c r="D86" s="63"/>
+    </row>
+    <row r="87" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="C87" s="63" t="s">
+        <v>313</v>
+      </c>
+      <c r="D87" s="63"/>
+    </row>
+    <row r="88" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="C88" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="89" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="C89" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="90" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="C90" s="63" t="s">
+        <v>327</v>
+      </c>
+      <c r="D90" s="63"/>
+    </row>
+    <row r="91" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="C91" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="92" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>328</v>
+      </c>
+      <c r="B92" t="s">
+        <v>178</v>
+      </c>
+      <c r="C92" s="125" t="s">
+        <v>204</v>
+      </c>
+      <c r="D92" s="125"/>
+      <c r="E92" s="125"/>
+      <c r="F92" s="125"/>
+      <c r="G92" s="125"/>
+      <c r="H92" s="125"/>
+      <c r="I92" s="125"/>
+      <c r="J92" s="125"/>
+      <c r="K92" s="125"/>
+      <c r="L92" s="125"/>
+      <c r="M92" s="125"/>
+      <c r="N92" s="125"/>
+      <c r="O92" s="125"/>
+      <c r="P92" s="125"/>
+    </row>
+    <row r="93" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="C93" s="125" t="s">
+        <v>205</v>
+      </c>
+      <c r="D93" s="125"/>
+      <c r="E93" s="125"/>
+      <c r="F93" s="125"/>
+      <c r="G93" s="125"/>
+      <c r="H93" s="125"/>
+      <c r="I93" s="125"/>
+      <c r="J93" s="125"/>
+      <c r="K93" s="125"/>
+      <c r="L93" s="125"/>
+      <c r="M93" s="125"/>
+      <c r="N93" s="125"/>
+      <c r="O93" s="125"/>
+      <c r="P93" s="125"/>
+    </row>
+    <row r="94" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="C94" s="125" t="s">
+        <v>206</v>
+      </c>
+      <c r="D94" s="125"/>
+      <c r="E94" s="125"/>
+      <c r="F94" s="125"/>
+      <c r="G94" s="125"/>
+      <c r="H94" s="125"/>
+      <c r="I94" s="125"/>
+      <c r="J94" s="125"/>
+      <c r="K94" s="125"/>
+      <c r="L94" s="125"/>
+      <c r="M94" s="125"/>
+      <c r="N94" s="125"/>
+      <c r="O94" s="125"/>
+      <c r="P94" s="125"/>
+    </row>
+    <row r="95" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="C95" s="125" t="s">
+        <v>207</v>
+      </c>
+      <c r="D95" s="125"/>
+      <c r="E95" s="125"/>
+      <c r="F95" s="125"/>
+      <c r="G95" s="125"/>
+      <c r="H95" s="125"/>
+      <c r="I95" s="125"/>
+      <c r="J95" s="125"/>
+      <c r="K95" s="125"/>
+      <c r="L95" s="125"/>
+      <c r="M95" s="125"/>
+      <c r="N95" s="125"/>
+      <c r="O95" s="125"/>
+      <c r="P95" s="125"/>
+    </row>
+    <row r="96" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="C96" s="125" t="s">
+        <v>208</v>
+      </c>
+      <c r="D96" s="125"/>
+      <c r="E96" s="125"/>
+      <c r="F96" s="125"/>
+      <c r="G96" s="125"/>
+      <c r="H96" s="125"/>
+      <c r="I96" s="125"/>
+      <c r="J96" s="125"/>
+      <c r="K96" s="125"/>
+      <c r="L96" s="125"/>
+      <c r="M96" s="125"/>
+      <c r="N96" s="125"/>
+      <c r="O96" s="125"/>
+      <c r="P96" s="125"/>
+    </row>
+    <row r="97" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="C97" s="125" t="s">
         <v>209</v>
       </c>
+      <c r="D97" s="125"/>
+      <c r="E97" s="125"/>
+      <c r="F97" s="125"/>
+      <c r="G97" s="125"/>
+      <c r="H97" s="125"/>
+      <c r="I97" s="125"/>
+      <c r="J97" s="125"/>
+      <c r="K97" s="125"/>
+      <c r="L97" s="125"/>
+      <c r="M97" s="125"/>
+      <c r="N97" s="125"/>
+      <c r="O97" s="125"/>
+      <c r="P97" s="125"/>
+    </row>
+    <row r="98" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>276</v>
+      </c>
+      <c r="B98" t="s">
+        <v>178</v>
+      </c>
+      <c r="C98" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="99" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="C99" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="100" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="C100" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="101" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="C101" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="102" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="C102" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="103" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>277</v>
+      </c>
+      <c r="B103" t="s">
+        <v>178</v>
+      </c>
+      <c r="C103" s="24" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="104" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="C104" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="105" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="C105" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="106" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="C106" t="s">
+        <v>281</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C42" r:id="rId1" xr:uid="{8C69B947-9BCD-463F-AA32-507C8EE29DAC}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -5105,7 +5743,7 @@
         <v>83</v>
       </c>
       <c r="J18" s="18" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -5438,7 +6076,7 @@
         <v>31</v>
       </c>
       <c r="P1" s="63" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="Q1" s="63"/>
       <c r="R1" s="63"/>
@@ -5457,7 +6095,7 @@
         <v>14</v>
       </c>
       <c r="P2" s="123" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="S2" s="77" t="s">
         <v>163</v>
@@ -21726,7 +22364,7 @@
         <v>83</v>
       </c>
       <c r="D18" s="18" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="E18" s="12">
         <v>1</v>

</xml_diff>